<commit_message>
update user managing function
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{5FF9A14E-D2E6-454F-9BA4-3D186F544A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CCF0A88-1793-4214-8223-34E7686505FB}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{5FF9A14E-D2E6-454F-9BA4-3D186F544A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6B6D40F-B6B3-40E2-BD9E-CE63C7554990}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="90" windowWidth="26910" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -138,7 +138,10 @@
     <t>Projektplan</t>
   </si>
   <si>
-    <t>Login, user controller/services</t>
+    <t>Logic: Login, user controller/services</t>
+  </si>
+  <si>
+    <t>Logic: admin management functions</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="#0&quot;:&quot;00"/>
-    <numFmt numFmtId="168" formatCode="[hh]:mm"/>
+    <numFmt numFmtId="167" formatCode="[hh]:mm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -239,7 +242,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -560,7 +563,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -590,7 +593,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(LEFT(B2:B101,LEN(B2:B101)-2)&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>1.2083333333333333</v>
+        <v>1.40625</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -774,8 +777,18 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="6"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="6">
+        <v>44289</v>
+      </c>
+      <c r="B15" s="9">
+        <v>445</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6"/>
@@ -4729,7 +4742,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>

<commit_message>
Merged logic with model, pw-issue fixed
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDrive - uibk.ac.at\Studium\Bachelor_4. Semester\PS Software Engineering\g6t1\documents\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{5FF9A14E-D2E6-454F-9BA4-3D186F544A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E043D211-95F3-433C-A746-59FD3E0F733C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="90" windowWidth="26910" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Logic: game stats</t>
+  </si>
+  <si>
+    <t>Link logic with db-model</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -596,7 +599,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(LEFT(B2:B101,LEN(B2:B101)-2)&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>1.4479166666666667</v>
+        <v>1.6145833333333333</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -798,7 +801,7 @@
         <v>44291</v>
       </c>
       <c r="B16" s="9">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -806,16 +809,20 @@
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16">
-        <v>1100</v>
-      </c>
-      <c r="F16">
-        <v>1200</v>
-      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="6"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="6">
+        <v>44294</v>
+      </c>
+      <c r="B17" s="9">
+        <v>200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6"/>

</xml_diff>

<commit_message>
update game logic + TermsServiceTest
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5663E17-F72B-42E4-933C-82E37A910730}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7EF56353-9719-4D35-A6F7-69AEBF7010C7}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="90" windowWidth="26910" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -572,7 +572,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -602,7 +602,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(LEFT(B2:B101,LEN(B2:B101)-2)&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>1.78125</v>
+        <v>1.9826388888888891</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -842,11 +842,29 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="6">
+        <v>44298</v>
+      </c>
+      <c r="B19" s="9">
+        <v>350</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6">
+        <v>44298</v>
+      </c>
+      <c r="B20" s="9">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">

</xml_diff>

<commit_message>
game creation and starting
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEB2C73A-5154-42BE-955E-9449FDBB9F03}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B44E148-A796-41C6-A461-53225C97A792}"/>
   <bookViews>
-    <workbookView xWindow="17775" yWindow="405" windowWidth="26910" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="8640" yWindow="285" windowWidth="21090" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -584,7 +584,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>4.3784722222222223</v>
+        <v>5.2118055555555554</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1018,16 +1018,46 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="6"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="6">
+        <v>44314</v>
+      </c>
+      <c r="B31" s="9">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="6"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="6">
+        <v>44315</v>
+      </c>
+      <c r="B32" s="9">
+        <v>500</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="6"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="6">
+        <v>44317</v>
+      </c>
+      <c r="B33" s="9">
+        <v>1400</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="6"/>

</xml_diff>

<commit_message>
We thought we were smarter than the Bugs.
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{759D87BE-E3B3-4894-AD81-8C18839543FF}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDFF9F3B-ADC8-4646-B191-4BD65FE76C2A}"/>
   <bookViews>
-    <workbookView xWindow="25935" yWindow="180" windowWidth="25155" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="11475" yWindow="180" windowWidth="25155" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
   <si>
     <t>Datum</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t xml:space="preserve">Game creation &amp; start </t>
+  </si>
+  <si>
+    <t>Game creation &amp; start debugging</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -620,7 +623,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>6.1493055555555562</v>
+        <v>6.5659722222222232</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1112,7 +1115,7 @@
         <v>44323</v>
       </c>
       <c r="B37" s="9">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1122,12 +1125,32 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="6"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="6">
+        <v>44416</v>
+      </c>
+      <c r="B38" s="9">
+        <v>400</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="6"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="6">
+        <v>44417</v>
+      </c>
+      <c r="B39" s="9">
+        <v>400</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="6"/>

</xml_diff>

<commit_message>
code cleanup & bugfix in user management
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDFF9F3B-ADC8-4646-B191-4BD65FE76C2A}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5597C59-713C-4FE3-A453-826ED88F6065}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="180" windowWidth="25155" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="2655" yWindow="225" windowWidth="25155" windowHeight="20565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Game creation &amp; start debugging</t>
+  </si>
+  <si>
+    <t>code cleanup, document &amp; bugfix</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -623,7 +626,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>6.5659722222222232</v>
+        <v>7.0243055555555562</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1054,7 +1057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="A33" s="6">
         <v>44317</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" s="6">
         <v>44318</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6">
       <c r="A35" s="6">
         <v>44319</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="A36" s="6">
         <v>44322</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6">
       <c r="A37" s="6">
         <v>44323</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6">
       <c r="A38" s="6">
         <v>44416</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:6">
       <c r="A39" s="6">
         <v>44417</v>
       </c>
@@ -1152,39 +1155,73 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="6"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="6"/>
+    <row r="40" spans="1:6">
+      <c r="A40" s="6">
+        <v>44326</v>
+      </c>
+      <c r="B40" s="9">
+        <v>300</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6">
+        <v>44326</v>
+      </c>
+      <c r="B41" s="9">
+        <v>130</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4">
+    <row r="42" spans="1:6">
+      <c r="A42" s="6">
+        <v>44328</v>
+      </c>
+      <c r="B42" s="9">
+        <v>630</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42">
+        <v>1500</v>
+      </c>
+      <c r="F42">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="6"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="A44" s="6"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:6">
       <c r="A45" s="6"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:6">
       <c r="A46" s="6"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:6">
       <c r="A47" s="6"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:6">
       <c r="A48" s="6"/>
       <c r="D48" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fixes in Topic & User hub
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{798BACC0-73C6-4BAA-910C-8F62EBAB0101}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBCEFF03-09C1-43E9-907B-EFD21EDA7658}"/>
   <bookViews>
     <workbookView xWindow="15435" yWindow="135" windowWidth="28335" windowHeight="20370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Fehlerbehebung</t>
+  </si>
+  <si>
+    <t>LV und GIT management</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
   <dimension ref="A1:K1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -638,7 +641,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>8.0034722222222232</v>
+        <v>8.2534722222222232</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1264,12 +1267,32 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="6"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="6">
+        <v>44347</v>
+      </c>
+      <c r="B47" s="9">
+        <v>200</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="6"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="6">
+        <v>44347</v>
+      </c>
+      <c r="B48" s="9">
+        <v>400</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="6"/>
@@ -5091,7 +5114,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>

<commit_message>
raspis: hide IPs and add authorization
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E68441AF-7CF6-410C-80AB-D35722ABB065}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBB02C8-9889-4617-85BB-34421DF791F9}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="135" windowWidth="33870" windowHeight="20370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="30" yWindow="15" windowWidth="28770" windowHeight="17370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -620,7 +620,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -650,7 +650,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>8.8368055555555571</v>
+        <v>8.9201388888888911</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1346,8 +1346,18 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="6"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="6">
+        <v>44353</v>
+      </c>
+      <c r="B52" s="9">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6"/>
@@ -5153,7 +5163,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>

<commit_message>
UI improvements & sign-up
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBB02C8-9889-4617-85BB-34421DF791F9}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67564A8-ADAA-4774-9EA7-116518E2EA57}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="15" windowWidth="28770" windowHeight="17370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
   <si>
     <t>Datum</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Improvements game join</t>
+  </si>
+  <si>
+    <t>UI and signup</t>
   </si>
 </sst>
 </file>
@@ -617,10 +620,10 @@
   <dimension ref="A1:K1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -650,7 +653,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>8.9201388888888911</v>
+        <v>9.315972222222225</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1360,8 +1363,18 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="6">
+        <v>44354</v>
+      </c>
+      <c r="B53" s="9">
+        <v>930</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="6"/>

</xml_diff>

<commit_message>
Softwarekonzept update & minor fixes
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67564A8-ADAA-4774-9EA7-116518E2EA57}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED14458C-D307-4EC6-A8D9-789064B5E4CC}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="15" windowWidth="28770" windowHeight="17370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>UI and signup</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -653,7 +656,7 @@
       </c>
       <c r="G1" s="12" cm="1">
         <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>9.315972222222225</v>
+        <v>9.4826388888888911</v>
       </c>
       <c r="H1" s="11"/>
       <c r="K1" s="10"/>
@@ -1377,8 +1380,18 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="6"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="6">
+        <v>44355</v>
+      </c>
+      <c r="B54" s="9">
+        <v>400</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="6"/>

</xml_diff>

<commit_message>
Softwarekonzept update & Abschlussbericht
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/sebastian_hepp-Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibkacat-my.sharepoint.com/personal/sebastian_hepp_student_uibk_ac_at/Documents/Studium/Bachelor_4. Semester/PS Software Engineering/g6t1/documents/zeitaufzeichnung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED14458C-D307-4EC6-A8D9-789064B5E4CC}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="13_ncr:1_{CF1D7CFD-8C75-4541-9FC9-885693EB3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00D5E4D3-05A8-48C2-AAC3-2E81B5AB0953}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="28770" windowHeight="17370" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="17805" yWindow="225" windowWidth="21990" windowHeight="20400" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Fehlerbehebung</t>
   </si>
   <si>
-    <t>LV und GIT management</t>
-  </si>
-  <si>
     <t>Improvements topic hub</t>
   </si>
   <si>
@@ -206,16 +203,18 @@
   <si>
     <t>update</t>
   </si>
+  <si>
+    <t>GIT management</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="166" formatCode="#0&quot;:&quot;00"/>
-    <numFmt numFmtId="167" formatCode="[hh]:mm"/>
+    <numFmt numFmtId="165" formatCode="#0&quot;:&quot;00"/>
+    <numFmt numFmtId="166" formatCode="[hh]:mm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -288,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -298,14 +297,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -620,28 +620,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:K1002"/>
+  <dimension ref="A1:K1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="8" customWidth="1"/>
     <col min="3" max="3" width="35.625" customWidth="1"/>
     <col min="4" max="4" width="48.75" customWidth="1"/>
+    <col min="5" max="5" width="11" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="31.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -650,22 +651,22 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="12" cm="1">
-        <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B101,LEN(B2:B101)-2)="",0,LEFT(B2:B101,LEN(B2:B101)-2))&amp;":"&amp;RIGHT(B2:B101,2)),0))</f>
-        <v>9.4826388888888911</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="K1" s="10"/>
+      <c r="G1" s="11" cm="1">
+        <f t="array" ref="G1">SUM(IFERROR(TIMEVALUE(IF(LEFT(B2:B102,LEN(B2:B102)-2)="",0,LEFT(B2:B102,LEN(B2:B102)-2))&amp;":"&amp;RIGHT(B2:B102,2)),0))</f>
+        <v>9.90625</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="6">
         <v>44256</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>200</v>
       </c>
       <c r="C2" t="s">
@@ -673,25 +674,33 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="E2" s="13">
+        <f>_xlfn.NUMBERVALUE(LEFT(B2,LEN(B2)-2)) + RIGHT(B2,2) / 60</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6">
         <v>44263</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3"/>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E59" si="0">_xlfn.NUMBERVALUE(LEFT(B3,LEN(B3)-2)) + RIGHT(B3,2) / 60</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="6">
         <v>44264</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>200</v>
       </c>
       <c r="C4" t="s">
@@ -699,13 +708,17 @@
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6">
         <v>44266</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>130</v>
       </c>
       <c r="C5" t="s">
@@ -713,13 +726,17 @@
       </c>
       <c r="D5" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="6">
         <v>44267</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>430</v>
       </c>
       <c r="C6" t="s">
@@ -727,13 +744,17 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="6">
         <v>44270</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>100</v>
       </c>
       <c r="C7" t="s">
@@ -741,13 +762,17 @@
       </c>
       <c r="D7" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6">
         <v>44272</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>300</v>
       </c>
       <c r="C8" t="s">
@@ -755,13 +780,17 @@
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6">
         <v>44273</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>300</v>
       </c>
       <c r="C9" t="s">
@@ -769,25 +798,33 @@
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="6">
         <v>44277</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3"/>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6">
         <v>44280</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>100</v>
       </c>
       <c r="C11" t="s">
@@ -795,13 +832,17 @@
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6">
         <v>44281</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>200</v>
       </c>
       <c r="C12" t="s">
@@ -809,13 +850,17 @@
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6">
         <v>44287</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>30</v>
       </c>
       <c r="C13" t="s">
@@ -824,12 +869,17 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="6">
         <v>44288</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>600</v>
       </c>
       <c r="C14" t="s">
@@ -837,13 +887,17 @@
       </c>
       <c r="D14" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="6">
         <v>44289</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>445</v>
       </c>
       <c r="C15" t="s">
@@ -851,13 +905,17 @@
       </c>
       <c r="D15" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6">
         <v>44291</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>300</v>
       </c>
       <c r="C16" t="s">
@@ -866,12 +924,16 @@
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="6">
         <v>44294</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>200</v>
       </c>
       <c r="C17" t="s">
@@ -880,12 +942,16 @@
       <c r="D17" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="6">
         <v>44297</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>400</v>
       </c>
       <c r="C18" t="s">
@@ -894,13 +960,17 @@
       <c r="D18" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="6">
         <v>44298</v>
       </c>
-      <c r="B19" s="9">
-        <v>350</v>
+      <c r="B19" s="8">
+        <v>330</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -908,24 +978,32 @@
       <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="6">
         <v>44298</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>100</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="6">
         <v>44302</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="8">
         <v>700</v>
       </c>
       <c r="C21" t="s">
@@ -934,12 +1012,16 @@
       <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="6">
         <v>44303</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="8">
         <v>300</v>
       </c>
       <c r="C22" t="s">
@@ -948,12 +1030,16 @@
       <c r="D22" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="6">
         <v>44303</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="8">
         <v>530</v>
       </c>
       <c r="C23" t="s">
@@ -962,12 +1048,16 @@
       <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="6">
         <v>44305</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>500</v>
       </c>
       <c r="C24" t="s">
@@ -976,12 +1066,16 @@
       <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="6">
         <v>44306</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>30</v>
       </c>
       <c r="C25" t="s">
@@ -990,12 +1084,16 @@
       <c r="D25" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="6">
         <v>44309</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>1000</v>
       </c>
       <c r="C26" t="s">
@@ -1004,12 +1102,16 @@
       <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="6">
         <v>44310</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="8">
         <v>1200</v>
       </c>
       <c r="C27" t="s">
@@ -1018,12 +1120,16 @@
       <c r="D27" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="6">
         <v>44311</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="8">
         <v>600</v>
       </c>
       <c r="C28" t="s">
@@ -1032,12 +1138,16 @@
       <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="6">
         <v>44312</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>600</v>
       </c>
       <c r="C29" t="s">
@@ -1046,24 +1156,32 @@
       <c r="D29" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="6">
         <v>44312</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="8">
         <v>200</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="6">
         <v>44314</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="8">
         <v>100</v>
       </c>
       <c r="C31" t="s">
@@ -1072,12 +1190,16 @@
       <c r="D31" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="6">
         <v>44315</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>500</v>
       </c>
       <c r="C32" t="s">
@@ -1086,12 +1208,16 @@
       <c r="D32" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="6">
         <v>44317</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>1400</v>
       </c>
       <c r="C33" t="s">
@@ -1100,12 +1226,16 @@
       <c r="D33" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="6">
         <v>44318</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>300</v>
       </c>
       <c r="C34" t="s">
@@ -1114,12 +1244,16 @@
       <c r="D34" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="6">
         <v>44319</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>1000</v>
       </c>
       <c r="C35" t="s">
@@ -1128,12 +1262,16 @@
       <c r="D35" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="6">
         <v>44322</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="8">
         <v>230</v>
       </c>
       <c r="C36" t="s">
@@ -1142,12 +1280,16 @@
       <c r="D36" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="6">
         <v>44323</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="8">
         <v>900</v>
       </c>
       <c r="C37" t="s">
@@ -1156,12 +1298,16 @@
       <c r="D37" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="6">
         <v>44416</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>400</v>
       </c>
       <c r="C38" t="s">
@@ -1170,12 +1316,16 @@
       <c r="D38" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="6">
         <v>44417</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>400</v>
       </c>
       <c r="C39" t="s">
@@ -1184,12 +1334,16 @@
       <c r="D39" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="6">
         <v>44326</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>300</v>
       </c>
       <c r="C40" t="s">
@@ -1198,24 +1352,32 @@
       <c r="D40" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="6">
         <v>44326</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="8">
         <v>130</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="6">
         <v>44328</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="8">
         <v>630</v>
       </c>
       <c r="C42" t="s">
@@ -1224,12 +1386,16 @@
       <c r="D42" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="6">
         <v>44329</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="8">
         <v>1300</v>
       </c>
       <c r="C43" t="s">
@@ -1238,12 +1404,16 @@
       <c r="D43" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="6">
         <v>44334</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="8">
         <v>300</v>
       </c>
       <c r="C44" t="s">
@@ -1252,12 +1422,16 @@
       <c r="D44" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="6">
         <v>44342</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="8">
         <v>100</v>
       </c>
       <c r="C45" t="s">
@@ -1266,12 +1440,16 @@
       <c r="D45" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="6">
         <v>44345</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="8">
         <v>630</v>
       </c>
       <c r="C46" t="s">
@@ -1280,55 +1458,69 @@
       <c r="D46" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="6">
         <v>44347</v>
       </c>
-      <c r="B47" s="9">
-        <v>200</v>
+      <c r="B47" s="8">
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="6">
         <v>44347</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="8">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="6">
+        <v>44347</v>
+      </c>
+      <c r="B49" s="8">
         <v>400</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="6">
-        <v>44351</v>
-      </c>
-      <c r="B49" s="9">
-        <v>200</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>39</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="6">
-        <v>44352</v>
-      </c>
-      <c r="B50" s="9">
-        <v>500</v>
+        <v>44351</v>
+      </c>
+      <c r="B50" s="8">
+        <v>200</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1336,100 +1528,186 @@
       <c r="D50" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="6">
         <v>44352</v>
       </c>
-      <c r="B51" s="9">
-        <v>700</v>
+      <c r="B51" s="8">
+        <v>500</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>40</v>
+      </c>
+      <c r="E51" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="6">
-        <v>44353</v>
-      </c>
-      <c r="B52" s="9">
-        <v>200</v>
+        <v>44352</v>
+      </c>
+      <c r="B52" s="8">
+        <v>700</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>42</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="6">
-        <v>44354</v>
-      </c>
-      <c r="B53" s="9">
-        <v>930</v>
+        <v>44353</v>
+      </c>
+      <c r="B53" s="8">
+        <v>200</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="6">
+        <v>44354</v>
+      </c>
+      <c r="B54" s="8">
+        <v>930</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="6">
+        <v>44355</v>
+      </c>
+      <c r="B55" s="8">
+        <v>400</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="6">
-        <v>44355</v>
-      </c>
-      <c r="B54" s="9">
+      <c r="E55" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="6">
+        <v>44358</v>
+      </c>
+      <c r="B56" s="8">
         <v>400</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="6"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="6"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="6"/>
+      <c r="D56" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="6">
+        <v>44359</v>
+      </c>
+      <c r="B57" s="8">
+        <v>500</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
       <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="6"/>
+      <c r="E57" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="6">
+        <v>44360</v>
+      </c>
+      <c r="B58" s="8">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
       <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="6"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E58" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="6">
+        <v>44360</v>
+      </c>
+      <c r="B59" s="8">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="6"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" s="6"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" s="6"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" s="6"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" s="6"/>
       <c r="D64" s="3"/>
     </row>
@@ -5182,7 +5460,11 @@
       <c r="D1001" s="3"/>
     </row>
     <row r="1002" spans="1:4">
-      <c r="A1002" s="2"/>
+      <c r="A1002" s="6"/>
+      <c r="D1002" s="3"/>
+    </row>
+    <row r="1003" spans="1:4">
+      <c r="A1003" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5194,7 +5476,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1001</xm:sqref>
+          <xm:sqref>C2:C1002</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>